<commit_message>
Updated Technical Analysis Report
</commit_message>
<xml_diff>
--- a/Technical Analysis Report - Enock.xlsx
+++ b/Technical Analysis Report - Enock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Corporate Training 2020\IIHT\From Praful\Yaksha Assignment\Assignment 1\Junior FSE PA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8A52E2-81AC-43A9-AAFB-47BBF98A9260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EDFEEC-5AD5-4033-8971-CA7FEEAFED07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5C6A7020-5E6E-C347-BE85-C8E642C78FD7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="178">
   <si>
     <t xml:space="preserve">Problem Statement </t>
   </si>
@@ -313,12 +313,6 @@
   </si>
   <si>
     <t>setUp</t>
-  </si>
-  <si>
-    <t>testGiftOrdersSuccess</t>
-  </si>
-  <si>
-    <t>testGiftOrderFailed</t>
   </si>
   <si>
     <t>Git Hub link</t>
@@ -597,12 +591,84 @@
   <si>
     <t>add comment</t>
   </si>
+  <si>
+    <t>testViewAllPosts</t>
+  </si>
+  <si>
+    <t>testViewAllPostsCase1</t>
+  </si>
+  <si>
+    <t>testSavePostsTestCase2</t>
+  </si>
+  <si>
+    <t>testAddPost</t>
+  </si>
+  <si>
+    <t>testAddComments</t>
+  </si>
+  <si>
+    <t>testSavePosts</t>
+  </si>
+  <si>
+    <t>testSaveComments</t>
+  </si>
+  <si>
+    <t>testViewAllDiscussions</t>
+  </si>
+  <si>
+    <t>testViewAllDiscussions1</t>
+  </si>
+  <si>
+    <t>testPostSuccess</t>
+  </si>
+  <si>
+    <t>testPostFailed</t>
+  </si>
+  <si>
+    <t>testCommentSuccess</t>
+  </si>
+  <si>
+    <t>testCommentFailed</t>
+  </si>
+  <si>
+    <t>testDiscussionSuccess</t>
+  </si>
+  <si>
+    <t>testDiscussionFailed</t>
+  </si>
+  <si>
+    <t>testCommentServiceImplTest</t>
+  </si>
+  <si>
+    <t>testViewAllCommentsImplTest</t>
+  </si>
+  <si>
+    <t>testViewAllCommentsImplTest1</t>
+  </si>
+  <si>
+    <t>testViewAllCommentsImplTest2</t>
+  </si>
+  <si>
+    <t>testSaveCommentsImplTest</t>
+  </si>
+  <si>
+    <t>testViewAllPostsImplTest</t>
+  </si>
+  <si>
+    <t>testViewAllPostsImplTest1</t>
+  </si>
+  <si>
+    <t>testViewAllPostsImplTest2</t>
+  </si>
+  <si>
+    <t>testSavePostsImplTest</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -757,6 +823,12 @@
       <color rgb="FFFF0000"/>
       <name val="Candara"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1126,7 +1198,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1383,6 +1455,7 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2253,8 +2326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC40B214-6783-784B-BE9B-36024B3C33AC}">
   <dimension ref="A1:W47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2265,9 +2338,13 @@
     <col min="4" max="4" width="32" customWidth="1"/>
     <col min="5" max="5" width="38.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.125" customWidth="1"/>
-    <col min="7" max="7" width="20.25" customWidth="1"/>
-    <col min="8" max="8" width="23.375" customWidth="1"/>
-    <col min="9" max="9" width="25.25" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="8" max="8" width="29.125" customWidth="1"/>
+    <col min="9" max="9" width="29.5" customWidth="1"/>
+    <col min="10" max="10" width="25.75" customWidth="1"/>
+    <col min="11" max="11" width="21.625" customWidth="1"/>
+    <col min="12" max="12" width="21.125" customWidth="1"/>
+    <col min="13" max="14" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
@@ -2327,10 +2404,10 @@
     </row>
     <row r="5" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A5" s="40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C5" s="52"/>
       <c r="D5" s="52"/>
@@ -2441,18 +2518,18 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -2461,18 +2538,18 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -2648,35 +2725,93 @@
       <c r="C31" t="s">
         <v>76</v>
       </c>
+      <c r="D31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" t="s">
+        <v>155</v>
+      </c>
+      <c r="F31" t="s">
+        <v>156</v>
+      </c>
+      <c r="G31" t="s">
+        <v>157</v>
+      </c>
+      <c r="H31" t="s">
+        <v>158</v>
+      </c>
+      <c r="I31" t="s">
+        <v>159</v>
+      </c>
+      <c r="J31" t="s">
+        <v>154</v>
+      </c>
+      <c r="K31" t="s">
+        <v>155</v>
+      </c>
+      <c r="L31" t="s">
+        <v>160</v>
+      </c>
+      <c r="M31" t="s">
+        <v>161</v>
+      </c>
+      <c r="N31" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" t="s">
+        <v>175</v>
+      </c>
+      <c r="D32" t="s">
+        <v>176</v>
+      </c>
+      <c r="E32" t="s">
+        <v>177</v>
+      </c>
+      <c r="F32" s="96" t="s">
+        <v>169</v>
+      </c>
+      <c r="G32" s="96" t="s">
+        <v>170</v>
+      </c>
+      <c r="H32" t="s">
+        <v>171</v>
+      </c>
+      <c r="I32" t="s">
+        <v>172</v>
+      </c>
+      <c r="J32" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
@@ -2684,13 +2819,25 @@
         <v>78</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>163</v>
       </c>
       <c r="D37" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="E37" t="s">
+        <v>165</v>
+      </c>
+      <c r="F37" t="s">
+        <v>166</v>
+      </c>
+      <c r="G37" t="s">
+        <v>167</v>
+      </c>
+      <c r="H37" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
@@ -2716,7 +2863,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2729,10 +2876,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C1" s="28" t="s">
         <v>57</v>
@@ -2744,13 +2891,13 @@
         <v>60</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
       <c r="B2" s="31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="28"/>
@@ -2759,10 +2906,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C3" s="21">
         <v>0</v>
@@ -2778,7 +2925,7 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="54"/>
       <c r="B4" s="36" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C4" s="37">
         <v>1</v>
@@ -2794,7 +2941,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="54"/>
       <c r="B5" s="38" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" s="21">
         <v>0</v>
@@ -2810,7 +2957,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="54"/>
       <c r="B6" s="38" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C6" s="21">
         <v>0</v>
@@ -2826,7 +2973,7 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="54"/>
       <c r="B7" s="35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C7" s="21">
         <v>0</v>
@@ -2842,7 +2989,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="54"/>
       <c r="B8" s="39" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C8" s="37">
         <v>1</v>
@@ -2858,7 +3005,7 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="54"/>
       <c r="B9" s="39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C9" s="37">
         <v>1</v>
@@ -2874,7 +3021,7 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="54"/>
       <c r="B10" s="38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C10" s="21">
         <v>0</v>
@@ -2890,7 +3037,7 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="54"/>
       <c r="B11" s="39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C11" s="37">
         <v>1</v>
@@ -2906,7 +3053,7 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="54"/>
       <c r="B12" s="35" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C12" s="21">
         <v>0</v>
@@ -2922,7 +3069,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="54"/>
       <c r="B13" s="35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C13" s="21">
         <v>0</v>
@@ -2938,7 +3085,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="54"/>
       <c r="B14" s="38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C14" s="21">
         <v>0</v>
@@ -2954,7 +3101,7 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="54"/>
       <c r="B15" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C15" s="21">
         <v>0</v>
@@ -2970,7 +3117,7 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="54"/>
       <c r="B16" s="38" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C16" s="21">
         <v>0</v>
@@ -2986,7 +3133,7 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="54"/>
       <c r="B17" s="35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C17" s="21">
         <v>0</v>
@@ -3002,7 +3149,7 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="54"/>
       <c r="B18" s="38" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C18" s="21">
         <v>0</v>
@@ -3018,7 +3165,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="55"/>
       <c r="B19" s="35" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C19" s="21">
         <v>0</v>
@@ -3033,7 +3180,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B20" s="56"/>
       <c r="C20" s="56"/>
@@ -3068,16 +3215,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>84</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3085,13 +3232,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C2" s="22">
         <v>43985</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3099,13 +3246,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C3" s="22">
         <v>43985</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3113,13 +3260,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C4" s="22">
         <v>43986</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3127,13 +3274,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C5" s="22">
         <v>43986</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3141,13 +3288,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>93</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3155,13 +3302,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>96</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3169,13 +3316,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C8" s="22">
         <v>43990</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3183,13 +3330,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C9" s="22">
         <v>43990</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3197,13 +3344,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C10" s="26">
         <v>43990</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -3226,7 +3373,7 @@
   <sheetData>
     <row r="3" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C3" s="58" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D3" s="58"/>
       <c r="E3" s="58"/>
@@ -3252,7 +3399,7 @@
     </row>
     <row r="6" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C6" s="59" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D6" s="59"/>
     </row>
@@ -3262,7 +3409,7 @@
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C9" s="59" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D9" s="59"/>
     </row>
@@ -3272,7 +3419,7 @@
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C12" s="59" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D12" s="59"/>
     </row>
@@ -3285,7 +3432,7 @@
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C15" s="59" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D15" s="59"/>
       <c r="H15" s="43"/>
@@ -3347,7 +3494,7 @@
   <sheetData>
     <row r="4" spans="5:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="E4" s="92" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F4" s="92"/>
       <c r="G4" s="92"/>
@@ -3359,11 +3506,11 @@
     </row>
     <row r="6" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E6" s="60" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F6" s="60"/>
       <c r="H6" s="90" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I6" s="90"/>
       <c r="J6" s="90"/>
@@ -3381,7 +3528,7 @@
     </row>
     <row r="9" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E9" s="60" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F9" s="60"/>
       <c r="H9" s="61"/>
@@ -3401,7 +3548,7 @@
     </row>
     <row r="12" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E12" s="60" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F12" s="60"/>
       <c r="H12" s="62"/>
@@ -3449,7 +3596,7 @@
     </row>
     <row r="19" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H19" s="63" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I19" s="63"/>
     </row>
@@ -3485,7 +3632,7 @@
   <sheetData>
     <row r="4" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="92" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C4" s="92"/>
       <c r="D4" s="92"/>
@@ -3498,7 +3645,7 @@
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E6" s="74" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F6" s="75"/>
       <c r="G6" s="75"/>
@@ -3516,7 +3663,7 @@
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C8" s="80" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D8" s="81"/>
       <c r="E8" s="81"/>
@@ -3565,7 +3712,7 @@
       <c r="G11" s="81"/>
       <c r="H11" s="81"/>
       <c r="L11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
@@ -3586,7 +3733,7 @@
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C16" s="69" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D16" s="70"/>
       <c r="E16" s="68"/>
@@ -3615,7 +3762,7 @@
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="69" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D20" s="70"/>
       <c r="E20" s="71"/>
@@ -3644,7 +3791,7 @@
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="64" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D25" s="65"/>
     </row>
@@ -3702,7 +3849,7 @@
   <sheetData>
     <row r="3" spans="3:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C3" s="93" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D3" s="94"/>
       <c r="E3" s="94"/>
@@ -3714,7 +3861,7 @@
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C5" s="63" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D5" s="63"/>
       <c r="F5" s="87"/>
@@ -3723,10 +3870,10 @@
       <c r="I5" s="88"/>
       <c r="J5" s="89"/>
       <c r="M5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.25">
@@ -3738,10 +3885,10 @@
       <c r="I6" s="88"/>
       <c r="J6" s="89"/>
       <c r="M6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="O6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="3:15" x14ac:dyDescent="0.25">
@@ -3802,7 +3949,7 @@
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" s="86" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D17" s="86"/>
       <c r="E17" s="86"/>

</xml_diff>